<commit_message>
kop en voettekst toegevoegd
</commit_message>
<xml_diff>
--- a/documenten/vrijdag-datamodel-database.xlsx
+++ b/documenten/vrijdag-datamodel-database.xlsx
@@ -450,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,5 +684,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CDatamodel Database</oddHeader>
+    <oddFooter>&amp;CDatum: 17-4-14
+Projectleden: Menno, Rick, Regilio, Sharif en Danny</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Uitleg per regel toegevoegd
</commit_message>
<xml_diff>
--- a/documenten/vrijdag-datamodel-database.xlsx
+++ b/documenten/vrijdag-datamodel-database.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -62,12 +62,6 @@
     <t>VarChar 2</t>
   </si>
   <si>
-    <t>Tabel: Teams</t>
-  </si>
-  <si>
-    <t>Tabel: Wedstrijden</t>
-  </si>
-  <si>
     <t>Teams_ID</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Tabel: Spelers</t>
-  </si>
-  <si>
     <t>Naam</t>
   </si>
   <si>
@@ -99,6 +90,69 @@
   </si>
   <si>
     <t>Default = Man</t>
+  </si>
+  <si>
+    <t>Tabel: tbl_teams</t>
+  </si>
+  <si>
+    <t>Tabel: tbl_wedstrijden</t>
+  </si>
+  <si>
+    <t>Tabel: tbl_spelers</t>
+  </si>
+  <si>
+    <t>Primary ID met sleutel</t>
+  </si>
+  <si>
+    <t>Team naam</t>
+  </si>
+  <si>
+    <t>Aantal doelpunten per team</t>
+  </si>
+  <si>
+    <t>Aantal spelers per team</t>
+  </si>
+  <si>
+    <t>Aantal keer gewonnen</t>
+  </si>
+  <si>
+    <t>Aantal keer verloren</t>
+  </si>
+  <si>
+    <t>Uitleg</t>
+  </si>
+  <si>
+    <t>Wedstrijd ID</t>
+  </si>
+  <si>
+    <t>Team ID, van tbl_teams</t>
+  </si>
+  <si>
+    <t>Wedstrijd tijd</t>
+  </si>
+  <si>
+    <t>De zaal van de wedstrijd</t>
+  </si>
+  <si>
+    <t>Aantal doelpunten per wedstrijd</t>
+  </si>
+  <si>
+    <t>Speler ID's</t>
+  </si>
+  <si>
+    <t>Speler namen</t>
+  </si>
+  <si>
+    <t>Speler leeftijden</t>
+  </si>
+  <si>
+    <t>Speler geslacht</t>
+  </si>
+  <si>
+    <t>Teams ID van _tbl_teams</t>
+  </si>
+  <si>
+    <t>Aantal doelpunten per speler</t>
   </si>
 </sst>
 </file>
@@ -448,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,17 +513,21 @@
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -482,8 +540,11 @@
       <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -494,8 +555,11 @@
       <c r="D3" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -508,8 +572,11 @@
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -518,8 +585,11 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -528,8 +598,11 @@
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -538,21 +611,27 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>7</v>
@@ -560,10 +639,13 @@
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
@@ -572,22 +654,28 @@
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>9</v>
@@ -596,8 +684,11 @@
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
@@ -606,21 +697,27 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>7</v>
@@ -628,58 +725,76 @@
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
+      <c r="E22" s="3" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>